<commit_message>
Arquivos e alterações auxiliares
</commit_message>
<xml_diff>
--- a/codigos/comparacao_resultados.xlsx
+++ b/codigos/comparacao_resultados.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unbbr-my.sharepoint.com/personal/211028972_aluno_unb_br/Documents/tcc_organizacao/codigos/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_23F921ED3B1B08143B2C4C0D7515485D681896EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90A77875-0DA9-4495-9156-B16032F6E3F7}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -22,28 +28,28 @@
     <t>disciplina</t>
   </si>
   <si>
-    <t>docente_dep</t>
-  </si>
-  <si>
-    <t>preferencia_dep</t>
-  </si>
-  <si>
-    <t>docente_pli</t>
-  </si>
-  <si>
-    <t>preferencia_pli</t>
-  </si>
-  <si>
-    <t>docente</t>
-  </si>
-  <si>
-    <t>preferencia</t>
-  </si>
-  <si>
-    <t>docente_ag</t>
-  </si>
-  <si>
-    <t>preferencia_ag</t>
+    <t>dep_docente</t>
+  </si>
+  <si>
+    <t>dep_preferencia</t>
+  </si>
+  <si>
+    <t>pli_docente</t>
+  </si>
+  <si>
+    <t>pli_preferencia</t>
+  </si>
+  <si>
+    <t>aco_docente</t>
+  </si>
+  <si>
+    <t>aco_preferencia</t>
+  </si>
+  <si>
+    <t>ag_docente</t>
+  </si>
+  <si>
+    <t>ag_preferencia</t>
   </si>
   <si>
     <t>EST0001_01</t>
@@ -349,8 +355,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,13 +419,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -457,7 +471,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -491,6 +505,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -525,9 +540,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -700,14 +716,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -739,7 +769,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -759,19 +789,19 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="H2">
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="J2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -797,13 +827,13 @@
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="J3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -835,7 +865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -867,7 +897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -887,7 +917,7 @@
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="H6">
         <v>3</v>
@@ -899,7 +929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -925,13 +955,13 @@
         <v>3</v>
       </c>
       <c r="I7" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="J7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -951,19 +981,19 @@
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="H8">
         <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="J8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -983,19 +1013,19 @@
         <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H9">
         <v>3</v>
       </c>
       <c r="I9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1015,19 +1045,19 @@
         <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="H10">
         <v>3</v>
       </c>
       <c r="I10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1053,13 +1083,13 @@
         <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J11">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1079,19 +1109,19 @@
         <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H12">
         <v>3</v>
       </c>
       <c r="I12" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="J12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1117,13 +1147,13 @@
         <v>3</v>
       </c>
       <c r="I13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J13">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1149,13 +1179,13 @@
         <v>3</v>
       </c>
       <c r="I14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1175,19 +1205,19 @@
         <v>3</v>
       </c>
       <c r="G15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H15">
         <v>3</v>
       </c>
       <c r="I15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="J15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1207,19 +1237,19 @@
         <v>3</v>
       </c>
       <c r="G16" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H16">
         <v>3</v>
       </c>
       <c r="I16" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="J16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1239,19 +1269,19 @@
         <v>3</v>
       </c>
       <c r="G17" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="H17">
         <v>3</v>
       </c>
       <c r="I17" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="J17">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1277,13 +1307,13 @@
         <v>3</v>
       </c>
       <c r="I18" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="J18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1303,19 +1333,19 @@
         <v>3</v>
       </c>
       <c r="G19" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="H19">
         <v>3</v>
       </c>
       <c r="I19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J19">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1335,19 +1365,19 @@
         <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="H20">
         <v>3</v>
       </c>
       <c r="I20" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="J20">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1367,19 +1397,19 @@
         <v>3</v>
       </c>
       <c r="G21" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H21">
         <v>3</v>
       </c>
       <c r="I21" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="J21">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1399,19 +1429,19 @@
         <v>3</v>
       </c>
       <c r="G22" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H22">
         <v>3</v>
       </c>
       <c r="I22" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="J22">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1431,19 +1461,19 @@
         <v>3</v>
       </c>
       <c r="G23" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="H23">
         <v>3</v>
       </c>
       <c r="I23" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="J23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1463,19 +1493,19 @@
         <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="H24">
         <v>3</v>
       </c>
       <c r="I24" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="J24">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1495,19 +1525,19 @@
         <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="H25">
         <v>3</v>
       </c>
       <c r="I25" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="J25">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1527,19 +1557,19 @@
         <v>3</v>
       </c>
       <c r="G26" t="s">
+        <v>84</v>
+      </c>
+      <c r="H26">
+        <v>3</v>
+      </c>
+      <c r="I26" t="s">
         <v>98</v>
       </c>
-      <c r="H26">
-        <v>3</v>
-      </c>
-      <c r="I26" t="s">
-        <v>93</v>
-      </c>
       <c r="J26">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1559,7 +1589,7 @@
         <v>3</v>
       </c>
       <c r="G27" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H27">
         <v>3</v>
@@ -1571,7 +1601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1591,19 +1621,19 @@
         <v>3</v>
       </c>
       <c r="G28" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="H28">
         <v>3</v>
       </c>
       <c r="I28" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="J28">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1623,19 +1653,19 @@
         <v>3</v>
       </c>
       <c r="G29" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="H29">
         <v>3</v>
       </c>
       <c r="I29" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="J29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1655,19 +1685,19 @@
         <v>3</v>
       </c>
       <c r="G30" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="H30">
         <v>3</v>
       </c>
       <c r="I30" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="J30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1693,13 +1723,13 @@
         <v>3</v>
       </c>
       <c r="I31" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="J31">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -1719,19 +1749,19 @@
         <v>3</v>
       </c>
       <c r="G32" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H32">
         <v>3</v>
       </c>
       <c r="I32" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="J32">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -1763,7 +1793,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1795,7 +1825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -1827,7 +1857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -1859,7 +1889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -1879,7 +1909,7 @@
         <v>3</v>
       </c>
       <c r="G37" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="H37">
         <v>3</v>
@@ -1891,7 +1921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -1911,7 +1941,7 @@
         <v>3</v>
       </c>
       <c r="G38" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="H38">
         <v>3</v>
@@ -1923,7 +1953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -1955,7 +1985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -1975,19 +2005,19 @@
         <v>3</v>
       </c>
       <c r="G40" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="H40">
         <v>3</v>
       </c>
       <c r="I40" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="J40">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -2007,7 +2037,7 @@
         <v>3</v>
       </c>
       <c r="G41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H41">
         <v>3</v>
@@ -2019,7 +2049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -2051,7 +2081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -2083,7 +2113,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -2115,7 +2145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -2147,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -2173,13 +2203,13 @@
         <v>2</v>
       </c>
       <c r="I46" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="J46">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -2199,7 +2229,7 @@
         <v>3</v>
       </c>
       <c r="G47" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="H47">
         <v>3</v>
@@ -2211,7 +2241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>56</v>
       </c>

</xml_diff>